<commit_message>
Processed Salesforce Current Translations
</commit_message>
<xml_diff>
--- a/scripts/trans/TranslationValidations/TranslationValidation.xlsx
+++ b/scripts/trans/TranslationValidations/TranslationValidation.xlsx
@@ -377,19 +377,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -504,13 +491,13 @@
         <v>Thông tin bổ sung</v>
       </c>
       <c r="O2" t="str">
-        <v>Misssing</v>
+        <v>CustomLabel$CEC_Shipment_Additional_Info</v>
       </c>
       <c r="P2" t="str">
-        <v>Misssing</v>
+        <v>CustomLabel</v>
       </c>
       <c r="Q2" t="str">
-        <v>Misssing</v>
+        <v>Additional Info</v>
       </c>
       <c r="R2" t="str">
         <v>shipmentIdentifier.xlsx</v>
@@ -563,13 +550,13 @@
         <v>Áp dụng</v>
       </c>
       <c r="O3" t="str">
-        <v>Misssing</v>
+        <v>CustomField$CEC_ShippingIdentifier__c.CEC_Applicable__c | CustomLabel$CEC_ShipmentIdentifier_Applicable</v>
       </c>
       <c r="P3" t="str">
-        <v>Misssing</v>
+        <v>CustomField | CustomLabel</v>
       </c>
       <c r="Q3" t="str">
-        <v>Misssing</v>
+        <v>Applicable</v>
       </c>
       <c r="R3" t="str">
         <v>shipmentIdentifier.xlsx</v>
@@ -619,13 +606,13 @@
         <v>Bạn phải chọn một hoặc nhiều định danh giao hàng để tiến hành.</v>
       </c>
       <c r="O4" t="str">
-        <v>Misssing</v>
+        <v>CustomLabel$CEC_Shipment_Non_Applicable_Error</v>
       </c>
       <c r="P4" t="str">
-        <v>Misssing</v>
+        <v>CustomLabel</v>
       </c>
       <c r="Q4" t="str">
-        <v>Misssing</v>
+        <v>You must select one or more shipment identifiers in order to proceed.</v>
       </c>
       <c r="R4" t="str">
         <v>shipmentIdentifier.xlsx</v>
@@ -643,6 +630,19 @@
   </sheetData>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:U4"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>